<commit_message>
Not clear what the changes were. Comit to clean-up branch.
</commit_message>
<xml_diff>
--- a/Docs/Cumming-Geothermal-Resource-Capacity-Power-Density-and-Risk-Tree-2019-10-10.xlsx
+++ b/Docs/Cumming-Geothermal-Resource-Capacity-Power-Density-and-Risk-Tree-2019-10-10.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irene\Dropbox (Personal)\PhD\Data-Analysis\PwrCap-PowerDensity-Public-GITREPO\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16B7AAF-5BCC-4DE0-AFC1-A42DEE3AA0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36" yWindow="6492" windowWidth="15480" windowHeight="6756" activeTab="2"/>
+    <workbookView xWindow="45972" yWindow="-12" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Lognormal MWe from Area" sheetId="5" r:id="rId1"/>
@@ -21,10 +27,22 @@
     <definedName name="Z_244A635C_1FC6_4F5E_A619_9E947BA21B2B_.wvu.PrintArea" localSheetId="0" hidden="1">'1. Lognormal MWe from Area'!$A$1:$N$61</definedName>
     <definedName name="Z_79A97261_3DC7_4D19_A3DF_02993B73D3BA_.wvu.PrintArea" localSheetId="1" hidden="1">'2. Tree-Capacity'!$A$48:$O$68</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="WBC - Personal View" guid="{79A97261-3DC7-4D19-A3DF-02993B73D3BA}" mergeInterval="0" personalView="1" maximized="1" windowWidth="931" windowHeight="616" activeSheetId="1"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1203,7 +1221,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2565,12 +2583,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3270,6 +3291,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-619D-4C61-BEF2-82E5A520A256}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3515,7 +3541,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4215,6 +4241,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AAE7-4603-B959-23A8E1329E5C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4476,7 +4507,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3133" name="Chart 1"/>
+        <xdr:cNvPr id="3133" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D0C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4508,7 +4545,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3134" name="Chart 2"/>
+        <xdr:cNvPr id="3134" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E0C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4545,7 +4588,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1043" name="Text Box 19"/>
+        <xdr:cNvPr id="1043" name="Text Box 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4784,7 +4833,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1044" name="Text Box 20"/>
+        <xdr:cNvPr id="1044" name="Text Box 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4918,7 +4973,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1045" name="Text Box 21"/>
+        <xdr:cNvPr id="1045" name="Text Box 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5033,7 +5094,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1046" name="Text Box 22"/>
+        <xdr:cNvPr id="1046" name="Text Box 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5120,7 +5187,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1047" name="Text Box 23"/>
+        <xdr:cNvPr id="1047" name="Text Box 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5209,7 +5282,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1048" name="Text Box 24"/>
+        <xdr:cNvPr id="1048" name="Text Box 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5315,7 +5394,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5687,14 +5772,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5704,19 +5789,19 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.87890625" customWidth="1"/>
+    <col min="3" max="3" width="11.87890625" customWidth="1"/>
+    <col min="4" max="4" width="10.3515625" customWidth="1"/>
+    <col min="5" max="5" width="10.52734375" customWidth="1"/>
+    <col min="6" max="6" width="9.64453125" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
-    <col min="15" max="17" width="9.109375" style="57" customWidth="1"/>
+    <col min="15" max="17" width="9.1171875" style="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="58" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="58" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="53"/>
       <c r="B1" s="54" t="s">
         <v>237</v>
@@ -5737,7 +5822,7 @@
       <c r="P1" s="57"/>
       <c r="Q1" s="57"/>
     </row>
-    <row r="2" spans="1:17" s="58" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="58" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="59"/>
       <c r="B2" s="60"/>
       <c r="C2" s="61"/>
@@ -5756,7 +5841,7 @@
       <c r="P2" s="57"/>
       <c r="Q2" s="57"/>
     </row>
-    <row r="3" spans="1:17" s="58" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="58" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="59"/>
       <c r="B3" s="233" t="s">
         <v>235</v>
@@ -5777,7 +5862,7 @@
       <c r="P3" s="57"/>
       <c r="Q3" s="57"/>
     </row>
-    <row r="4" spans="1:17" s="58" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="58" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="59"/>
       <c r="B4" s="236" t="s">
         <v>236</v>
@@ -5798,7 +5883,7 @@
       <c r="P4" s="57"/>
       <c r="Q4" s="57"/>
     </row>
-    <row r="5" spans="1:17" s="58" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="58" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="59"/>
       <c r="B5" s="239"/>
       <c r="C5" s="240"/>
@@ -5817,7 +5902,7 @@
       <c r="P5" s="57"/>
       <c r="Q5" s="57"/>
     </row>
-    <row r="6" spans="1:17" s="58" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="58" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="59"/>
       <c r="B6" s="64"/>
       <c r="C6" s="64"/>
@@ -5836,7 +5921,7 @@
       <c r="P6" s="57"/>
       <c r="Q6" s="57"/>
     </row>
-    <row r="7" spans="1:17" s="58" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="58" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="59"/>
       <c r="B7" s="65" t="s">
         <v>152</v>
@@ -5857,7 +5942,7 @@
       <c r="P7" s="57"/>
       <c r="Q7" s="57"/>
     </row>
-    <row r="8" spans="1:17" s="58" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="58" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="59"/>
       <c r="B8" s="233" t="s">
         <v>234</v>
@@ -5878,7 +5963,7 @@
       <c r="P8" s="57"/>
       <c r="Q8" s="57"/>
     </row>
-    <row r="9" spans="1:17" s="58" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="58" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="59"/>
       <c r="B9" s="63"/>
       <c r="C9" s="244" t="s">
@@ -5905,7 +5990,7 @@
       <c r="P9" s="57"/>
       <c r="Q9" s="57"/>
     </row>
-    <row r="10" spans="1:17" s="58" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="58" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="59"/>
       <c r="B10" s="67"/>
       <c r="C10" s="245" t="s">
@@ -5932,7 +6017,7 @@
       <c r="P10" s="57"/>
       <c r="Q10" s="57"/>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="59"/>
       <c r="B11" s="71" t="s">
         <v>157</v>
@@ -5965,7 +6050,7 @@
       <c r="M11" s="247"/>
       <c r="N11" s="62"/>
     </row>
-    <row r="12" spans="1:17" s="58" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="58" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="59"/>
       <c r="B12" s="74"/>
       <c r="C12" s="75"/>
@@ -5984,7 +6069,7 @@
       <c r="P12" s="57"/>
       <c r="Q12" s="57"/>
     </row>
-    <row r="13" spans="1:17" s="58" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="58" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="59"/>
       <c r="B13" s="61"/>
       <c r="C13" s="61"/>
@@ -6003,7 +6088,7 @@
       <c r="P13" s="57"/>
       <c r="Q13" s="57"/>
     </row>
-    <row r="14" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="67"/>
       <c r="B14" s="65" t="s">
         <v>160</v>
@@ -6024,7 +6109,7 @@
       <c r="P14" s="57"/>
       <c r="Q14" s="57"/>
     </row>
-    <row r="15" spans="1:17" s="58" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="58" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="67"/>
       <c r="B15" s="79"/>
       <c r="C15" s="80"/>
@@ -6043,7 +6128,7 @@
       <c r="P15" s="57"/>
       <c r="Q15" s="57"/>
     </row>
-    <row r="16" spans="1:17" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="67"/>
       <c r="B16" s="82"/>
       <c r="C16" s="60"/>
@@ -6067,7 +6152,7 @@
       <c r="N16" s="62"/>
       <c r="O16" s="78"/>
     </row>
-    <row r="17" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="67"/>
       <c r="B17" s="82"/>
       <c r="C17" s="60"/>
@@ -6084,7 +6169,7 @@
       <c r="N17" s="62"/>
       <c r="O17" s="78"/>
     </row>
-    <row r="18" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="67"/>
       <c r="B18" s="82" t="s">
         <v>161</v>
@@ -6103,7 +6188,7 @@
       <c r="N18" s="62"/>
       <c r="O18" s="78"/>
     </row>
-    <row r="19" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="67"/>
       <c r="B19" s="82"/>
       <c r="C19" s="60"/>
@@ -6132,7 +6217,7 @@
       <c r="N19" s="62"/>
       <c r="O19" s="78"/>
     </row>
-    <row r="20" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="67"/>
       <c r="B20" s="82"/>
       <c r="C20" s="60"/>
@@ -6149,7 +6234,7 @@
       <c r="N20" s="62"/>
       <c r="O20" s="78"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21" s="67"/>
       <c r="B21" s="87"/>
       <c r="C21" s="88" t="s">
@@ -6168,7 +6253,7 @@
       <c r="N21" s="62"/>
       <c r="O21" s="91"/>
     </row>
-    <row r="22" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="67"/>
       <c r="B22" s="87"/>
       <c r="C22" s="77"/>
@@ -6185,7 +6270,7 @@
       <c r="N22" s="62"/>
       <c r="O22" s="91"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23" s="67"/>
       <c r="B23" s="92"/>
       <c r="C23" s="93" t="s">
@@ -6209,7 +6294,7 @@
       <c r="N23" s="62"/>
       <c r="O23" s="91"/>
     </row>
-    <row r="24" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="67"/>
       <c r="B24" s="82"/>
       <c r="C24" s="84"/>
@@ -6248,7 +6333,7 @@
       <c r="N24" s="62"/>
       <c r="O24" s="78"/>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="67"/>
       <c r="B25" s="103" t="str">
         <f>"Area &gt; "&amp;(I19)&amp;"°C"</f>
@@ -6298,7 +6383,7 @@
       <c r="N25" s="62"/>
       <c r="O25" s="78"/>
     </row>
-    <row r="26" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="13.7" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="67"/>
       <c r="B26" s="103" t="str">
         <f>"Power Density "&amp;(I19)&amp;" to "&amp;(G19)&amp;" °C"</f>
@@ -6348,7 +6433,7 @@
       <c r="N26" s="107"/>
       <c r="O26" s="108"/>
     </row>
-    <row r="27" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="67"/>
       <c r="B27" s="103"/>
       <c r="C27" s="84"/>
@@ -6365,7 +6450,7 @@
       <c r="N27" s="107"/>
       <c r="O27" s="108"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28" s="67"/>
       <c r="B28" s="109" t="s">
         <v>124</v>
@@ -6413,7 +6498,7 @@
       </c>
       <c r="N28" s="114"/>
     </row>
-    <row r="29" spans="1:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="67"/>
       <c r="B29" s="104"/>
       <c r="C29" s="84"/>
@@ -6429,7 +6514,7 @@
       <c r="M29" s="101"/>
       <c r="N29" s="114"/>
     </row>
-    <row r="30" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="67"/>
       <c r="B30" s="65" t="s">
         <v>173</v>
@@ -6447,7 +6532,7 @@
       <c r="M30" s="101"/>
       <c r="N30" s="114"/>
     </row>
-    <row r="31" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="67"/>
       <c r="B31" s="53"/>
       <c r="C31" s="116"/>
@@ -6463,7 +6548,7 @@
       <c r="M31" s="119"/>
       <c r="N31" s="114"/>
     </row>
-    <row r="32" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="67"/>
       <c r="B32" s="120" t="s">
         <v>165</v>
@@ -6486,7 +6571,7 @@
       <c r="M32" s="102"/>
       <c r="N32" s="114"/>
     </row>
-    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="67"/>
       <c r="B33" s="120" t="s">
         <v>167</v>
@@ -6509,7 +6594,7 @@
       <c r="M33" s="102"/>
       <c r="N33" s="114"/>
     </row>
-    <row r="34" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="67"/>
       <c r="B34" s="109"/>
       <c r="C34" s="110"/>
@@ -6525,7 +6610,7 @@
       <c r="M34" s="113"/>
       <c r="N34" s="114"/>
     </row>
-    <row r="35" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="67"/>
       <c r="B35" s="104"/>
       <c r="C35" s="84"/>
@@ -6541,7 +6626,7 @@
       <c r="M35" s="101"/>
       <c r="N35" s="114"/>
     </row>
-    <row r="36" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="74"/>
       <c r="B36" s="123" t="s">
         <v>238</v>
@@ -6561,7 +6646,7 @@
       <c r="P36" s="198"/>
       <c r="Q36" s="198"/>
     </row>
-    <row r="37" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="13.7" x14ac:dyDescent="0.4">
       <c r="A37" s="128"/>
       <c r="B37" s="129"/>
       <c r="C37" s="77"/>
@@ -6592,7 +6677,7 @@
         <v>2.5132753913110153</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A38" s="58"/>
       <c r="B38" s="58"/>
       <c r="C38" s="58"/>
@@ -6623,7 +6708,7 @@
         <v>5.2370422542891388</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A39" s="58"/>
       <c r="B39" s="58"/>
       <c r="C39" s="58"/>
@@ -6654,7 +6739,7 @@
         <v>6.805642198285387</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A40" s="58"/>
       <c r="B40" s="58"/>
       <c r="C40" s="58"/>
@@ -6685,7 +6770,7 @@
         <v>8.0363862172287739</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A41" s="58"/>
       <c r="B41" s="58"/>
       <c r="C41" s="58"/>
@@ -6716,7 +6801,7 @@
         <v>9.1068418481343745</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A42" s="58"/>
       <c r="B42" s="58"/>
       <c r="C42" s="58"/>
@@ -6747,7 +6832,7 @@
         <v>10.08189906278824</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A43" s="58"/>
       <c r="B43" s="58"/>
       <c r="C43" s="58"/>
@@ -6778,7 +6863,7 @@
         <v>10.993647957545489</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A44" s="58"/>
       <c r="B44" s="58"/>
       <c r="C44" s="58"/>
@@ -6809,7 +6894,7 @@
         <v>11.860669785391494</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A45" s="58"/>
       <c r="B45" s="58"/>
       <c r="C45" s="58"/>
@@ -6840,7 +6925,7 @@
         <v>12.694850175232466</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A46" s="58"/>
       <c r="B46" s="58"/>
       <c r="C46" s="58"/>
@@ -6871,7 +6956,7 @@
         <v>13.504339622329141</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A47" s="58"/>
       <c r="B47" s="58"/>
       <c r="C47" s="58"/>
@@ -6902,7 +6987,7 @@
         <v>14.295025306526417</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A48" s="58"/>
       <c r="B48" s="58"/>
       <c r="C48" s="58"/>
@@ -6933,7 +7018,7 @@
         <v>15.071336294218234</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A49" s="58"/>
       <c r="B49" s="58"/>
       <c r="C49" s="58"/>
@@ -6964,7 +7049,7 @@
         <v>15.836716921638263</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A50" s="58"/>
       <c r="B50" s="58"/>
       <c r="C50" s="58"/>
@@ -6995,7 +7080,7 @@
         <v>16.59392122755991</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A51" s="58"/>
       <c r="B51" s="58"/>
       <c r="C51" s="58"/>
@@ -7026,7 +7111,7 @@
         <v>17.345204596849833</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A52" s="58"/>
       <c r="B52" s="58"/>
       <c r="C52" s="58"/>
@@ -7057,7 +7142,7 @@
         <v>18.092453272754625</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A53" s="58"/>
       <c r="B53" s="58"/>
       <c r="C53" s="58"/>
@@ -7088,7 +7173,7 @@
         <v>18.837274697129626</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A54" s="58"/>
       <c r="B54" s="58"/>
       <c r="C54" s="58"/>
@@ -7119,7 +7204,7 @@
         <v>19.581062263395861</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A55" s="58"/>
       <c r="B55" s="58"/>
       <c r="C55" s="58"/>
@@ -7150,7 +7235,7 @@
         <v>20.325042844063322</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A56" s="58"/>
       <c r="B56" s="58"/>
       <c r="C56" s="58"/>
@@ -7181,7 +7266,7 @@
         <v>21.070312417161144</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A57" s="58"/>
       <c r="B57" s="58"/>
       <c r="C57" s="58"/>
@@ -7212,7 +7297,7 @@
         <v>21.817863283073731</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A58" s="58"/>
       <c r="B58" s="58"/>
       <c r="C58" s="58"/>
@@ -7243,7 +7328,7 @@
         <v>22.568605221312392</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A59" s="58"/>
       <c r="B59" s="58"/>
       <c r="C59" s="58"/>
@@ -7274,7 +7359,7 @@
         <v>23.323382204960282</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A60" s="58"/>
       <c r="B60" s="58"/>
       <c r="C60" s="58"/>
@@ -7305,7 +7390,7 @@
         <v>24.082985809781174</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A61" s="58"/>
       <c r="B61" s="58"/>
       <c r="C61" s="58"/>
@@ -7336,7 +7421,7 @@
         <v>24.848166132096736</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="6.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B62" s="201"/>
       <c r="C62" s="201"/>
       <c r="D62" s="201"/>
@@ -7366,7 +7451,7 @@
         <v>25.619640808349519</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B63" s="58"/>
       <c r="C63" s="58"/>
       <c r="D63" s="58"/>
@@ -7396,7 +7481,7 @@
         <v>26.398102575039761</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B64" s="58"/>
       <c r="C64" s="58"/>
       <c r="D64" s="58"/>
@@ -7414,7 +7499,7 @@
       <c r="P64" s="132"/>
       <c r="R64" s="200"/>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B65" s="58"/>
       <c r="C65" s="58"/>
       <c r="D65" s="58"/>
@@ -7432,7 +7517,7 @@
       <c r="P65" s="132"/>
       <c r="R65" s="200"/>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B66" s="58"/>
       <c r="C66" s="58"/>
       <c r="D66" s="58"/>
@@ -7450,7 +7535,7 @@
       <c r="P66" s="132"/>
       <c r="R66" s="200"/>
     </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.4">
       <c r="O67"/>
       <c r="P67" s="132" t="e">
         <f>LOGINV(O67/100,$L$28,$M$28)*$L$11</f>
@@ -7465,23 +7550,23 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="68" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="O68"/>
       <c r="P68" s="132"/>
       <c r="R68" s="200"/>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.4">
       <c r="O69"/>
       <c r="P69" s="132"/>
       <c r="R69" s="200"/>
     </row>
-    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:18" x14ac:dyDescent="0.4">
       <c r="N70" s="58"/>
       <c r="O70" s="131"/>
       <c r="P70" s="132"/>
       <c r="R70" s="200"/>
     </row>
-    <row r="71" spans="2:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:18" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N71" s="58"/>
       <c r="O71" s="131">
         <v>28</v>
@@ -7499,7 +7584,7 @@
         <v>27.978671525142939</v>
       </c>
     </row>
-    <row r="72" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N72" s="58"/>
       <c r="O72" s="131">
         <v>29</v>
@@ -7517,7 +7602,7 @@
         <v>28.782093346784713</v>
       </c>
     </row>
-    <row r="73" spans="2:18" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:18" ht="6.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N73" s="58"/>
       <c r="O73" s="131">
         <v>30</v>
@@ -7535,7 +7620,7 @@
         <v>29.595140731401802</v>
       </c>
     </row>
-    <row r="74" spans="2:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N74" s="58"/>
       <c r="O74" s="131">
         <v>31</v>
@@ -7553,7 +7638,7 @@
         <v>30.41846344121555</v>
       </c>
     </row>
-    <row r="75" spans="2:18" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:18" ht="3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N75" s="58"/>
       <c r="O75" s="131">
         <v>32</v>
@@ -7571,7 +7656,7 @@
         <v>31.252715034431368</v>
       </c>
     </row>
-    <row r="76" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N76" s="58"/>
       <c r="O76" s="131">
         <v>33</v>
@@ -7589,7 +7674,7 @@
         <v>32.098556230490175</v>
       </c>
     </row>
-    <row r="77" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N77" s="58"/>
       <c r="O77" s="131">
         <v>34</v>
@@ -7607,7 +7692,7 @@
         <v>32.956658105127332</v>
       </c>
     </row>
-    <row r="78" spans="2:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N78" s="58"/>
       <c r="O78" s="131">
         <v>35</v>
@@ -7625,7 +7710,7 @@
         <v>33.827705171599739</v>
       </c>
     </row>
-    <row r="79" spans="2:18" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:18" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N79" s="58"/>
       <c r="O79" s="131">
         <v>36</v>
@@ -7643,7 +7728,7 @@
         <v>34.712398396989137</v>
       </c>
     </row>
-    <row r="80" spans="2:18" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:18" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N80" s="58"/>
       <c r="O80" s="131">
         <v>37</v>
@@ -7661,7 +7746,7 @@
         <v>35.611458197006584</v>
       </c>
     </row>
-    <row r="81" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N81" s="58"/>
       <c r="O81" s="131">
         <v>38</v>
@@ -7679,7 +7764,7 @@
         <v>36.525627448815548</v>
       </c>
     </row>
-    <row r="82" spans="14:18" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="14:18" ht="6.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N82" s="58"/>
       <c r="O82" s="131">
         <v>39</v>
@@ -7697,13 +7782,13 @@
         <v>37.4556745587672</v>
       </c>
     </row>
-    <row r="83" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N83" s="58"/>
       <c r="O83" s="131"/>
       <c r="P83" s="132"/>
       <c r="R83" s="200"/>
     </row>
-    <row r="84" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N84" s="58"/>
       <c r="O84" s="131">
         <v>40</v>
@@ -7721,7 +7806,7 @@
         <v>38.402396620397433</v>
       </c>
     </row>
-    <row r="85" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N85" s="58"/>
       <c r="O85" s="131">
         <v>41</v>
@@ -7739,7 +7824,7 @@
         <v>39.366622697426273</v>
       </c>
     </row>
-    <row r="86" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N86" s="58"/>
       <c r="O86" s="131">
         <v>42</v>
@@ -7757,7 +7842,7 @@
         <v>40.349217266729617</v>
       </c>
     </row>
-    <row r="87" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N87" s="58"/>
       <c r="O87" s="131">
         <v>43</v>
@@ -7775,7 +7860,7 @@
         <v>41.351083857267355</v>
       </c>
     </row>
-    <row r="88" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N88" s="58"/>
       <c r="O88" s="131">
         <v>44</v>
@@ -7793,7 +7878,7 @@
         <v>42.373168922724581</v>
       </c>
     </row>
-    <row r="89" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N89" s="58"/>
       <c r="O89" s="131">
         <v>45</v>
@@ -7811,7 +7896,7 @@
         <v>43.416465988163267</v>
       </c>
     </row>
-    <row r="90" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N90" s="58"/>
       <c r="O90" s="131">
         <v>46</v>
@@ -7829,7 +7914,7 @@
         <v>44.482020114321109</v>
       </c>
     </row>
-    <row r="91" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N91" s="58"/>
       <c r="O91" s="131">
         <v>47</v>
@@ -7847,7 +7932,7 @@
         <v>45.570932727394649</v>
       </c>
     </row>
-    <row r="92" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N92" s="58"/>
       <c r="O92" s="131">
         <v>48</v>
@@ -7865,7 +7950,7 @@
         <v>46.684366867293321</v>
       </c>
     </row>
-    <row r="93" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N93" s="58"/>
       <c r="O93" s="131">
         <v>49</v>
@@ -7883,7 +7968,7 @@
         <v>47.823552913568783</v>
       </c>
     </row>
-    <row r="94" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N94" s="58"/>
       <c r="O94" s="131">
         <v>50</v>
@@ -7901,7 +7986,7 @@
         <v>48.98979485566359</v>
       </c>
     </row>
-    <row r="95" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N95" s="58"/>
       <c r="O95" s="131">
         <v>51</v>
@@ -7919,7 +8004,7 @@
         <v>50.184477182979435</v>
       </c>
     </row>
-    <row r="96" spans="14:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="14:18" x14ac:dyDescent="0.4">
       <c r="N96" s="58"/>
       <c r="O96" s="131">
         <v>52</v>
@@ -7937,7 +8022,7 @@
         <v>51.409072480779912</v>
       </c>
     </row>
-    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:18" x14ac:dyDescent="0.4">
       <c r="N97" s="58"/>
       <c r="O97" s="131">
         <v>53</v>
@@ -7955,7 +8040,7 @@
         <v>52.665149830415018</v>
       </c>
     </row>
-    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B98" s="58"/>
       <c r="C98" s="58"/>
       <c r="D98" s="58"/>
@@ -7985,7 +8070,7 @@
         <v>53.954384127156935</v>
       </c>
     </row>
-    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B99" s="58"/>
       <c r="C99" s="58"/>
       <c r="D99" s="58"/>
@@ -8015,7 +8100,7 @@
         <v>55.278566446525609</v>
       </c>
     </row>
-    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B100" s="58"/>
       <c r="C100" s="58"/>
       <c r="D100" s="58"/>
@@ -8045,7 +8130,7 @@
         <v>56.63961561092713</v>
       </c>
     </row>
-    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B101" s="58"/>
       <c r="C101" s="58"/>
       <c r="D101" s="58"/>
@@ -8075,7 +8160,7 @@
         <v>58.039591133430648</v>
       </c>
     </row>
-    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B102" s="58"/>
       <c r="C102" s="58"/>
       <c r="D102" s="58"/>
@@ -8105,7 +8190,7 @@
         <v>59.480707745449799</v>
       </c>
     </row>
-    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B103" s="58"/>
       <c r="C103" s="58"/>
       <c r="D103" s="58"/>
@@ -8135,7 +8220,7 @@
         <v>60.965351751063743</v>
       </c>
     </row>
-    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B104" s="58"/>
       <c r="C104" s="58"/>
       <c r="D104" s="58"/>
@@ -8165,7 +8250,7 @@
         <v>62.496099494093642</v>
       </c>
     </row>
-    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B105" s="58"/>
       <c r="C105" s="58"/>
       <c r="D105" s="58"/>
@@ -8195,7 +8280,7 @@
         <v>64.075738276571471</v>
       </c>
     </row>
-    <row r="106" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B106" s="58"/>
       <c r="C106" s="58"/>
       <c r="D106" s="58"/>
@@ -8225,7 +8310,7 @@
         <v>65.707290131105722</v>
       </c>
     </row>
-    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B107" s="58"/>
       <c r="C107" s="58"/>
       <c r="D107" s="58"/>
@@ -8255,7 +8340,7 @@
         <v>67.394038927665704</v>
       </c>
     </row>
-    <row r="108" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B108" s="58"/>
       <c r="C108" s="58"/>
       <c r="D108" s="58"/>
@@ -8285,7 +8370,7 @@
         <v>69.139561391072661</v>
       </c>
     </row>
-    <row r="109" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B109" s="58"/>
       <c r="C109" s="58"/>
       <c r="D109" s="58"/>
@@ -8315,7 +8400,7 @@
         <v>70.947762723642768</v>
       </c>
     </row>
-    <row r="110" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B110" s="58"/>
       <c r="C110" s="58"/>
       <c r="D110" s="58"/>
@@ -8345,7 +8430,7 @@
         <v>72.822917674004543</v>
       </c>
     </row>
-    <row r="111" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B111" s="58"/>
       <c r="C111" s="58"/>
       <c r="D111" s="58"/>
@@ -8375,7 +8460,7 @@
         <v>74.769718075988081</v>
       </c>
     </row>
-    <row r="112" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B112" s="58"/>
       <c r="C112" s="58"/>
       <c r="D112" s="58"/>
@@ -8405,7 +8490,7 @@
         <v>76.793328111042641</v>
       </c>
     </row>
-    <row r="113" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B113" s="58"/>
       <c r="C113" s="58"/>
       <c r="D113" s="58"/>
@@ -8435,7 +8520,7 @@
         <v>78.899448837646318</v>
       </c>
     </row>
-    <row r="114" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B114" s="58"/>
       <c r="C114" s="58"/>
       <c r="D114" s="58"/>
@@ -8465,7 +8550,7 @@
         <v>81.094393900059828</v>
       </c>
     </row>
-    <row r="115" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B115" s="58"/>
       <c r="C115" s="58"/>
       <c r="D115" s="58"/>
@@ -8495,7 +8580,7 @@
         <v>83.385178801392144</v>
       </c>
     </row>
-    <row r="116" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B116" s="58"/>
       <c r="C116" s="58"/>
       <c r="D116" s="58"/>
@@ -8525,7 +8610,7 @@
         <v>85.779626736146199</v>
       </c>
     </row>
-    <row r="117" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B117" s="58"/>
       <c r="C117" s="58"/>
       <c r="D117" s="58"/>
@@ -8555,7 +8640,7 @@
         <v>88.286494771705435</v>
       </c>
     </row>
-    <row r="118" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B118" s="58"/>
       <c r="C118" s="58"/>
       <c r="D118" s="58"/>
@@ -8585,7 +8670,7 @@
         <v>90.915625211233063</v>
       </c>
     </row>
-    <row r="119" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B119" s="58"/>
       <c r="C119" s="58"/>
       <c r="D119" s="58"/>
@@ -8615,7 +8700,7 @@
         <v>93.678128352909425</v>
       </c>
     </row>
-    <row r="120" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B120" s="58"/>
       <c r="C120" s="58"/>
       <c r="D120" s="58"/>
@@ -8645,7 +8730,7 @@
         <v>96.586604711238138</v>
       </c>
     </row>
-    <row r="121" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B121" s="58"/>
       <c r="C121" s="58"/>
       <c r="D121" s="58"/>
@@ -8675,7 +8760,7 @@
         <v>99.655417270779409</v>
       </c>
     </row>
-    <row r="122" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B122" s="58"/>
       <c r="C122" s="58"/>
       <c r="D122" s="58"/>
@@ -8705,7 +8790,7 @@
         <v>102.90102777158899</v>
       </c>
     </row>
-    <row r="123" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B123" s="58"/>
       <c r="C123" s="58"/>
       <c r="D123" s="58"/>
@@ -8735,7 +8820,7 @@
         <v>106.34241577913686</v>
       </c>
     </row>
-    <row r="124" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B124" s="58"/>
       <c r="C124" s="58"/>
       <c r="D124" s="58"/>
@@ -8765,7 +8850,7 @@
         <v>110.0016059712832</v>
       </c>
     </row>
-    <row r="125" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B125" s="58"/>
       <c r="C125" s="58"/>
       <c r="D125" s="58"/>
@@ -8795,7 +8880,7 @@
         <v>113.90433860132389</v>
       </c>
     </row>
-    <row r="126" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B126" s="58"/>
       <c r="C126" s="58"/>
       <c r="D126" s="58"/>
@@ -8825,7 +8910,7 @@
         <v>118.08093190322626</v>
       </c>
     </row>
-    <row r="127" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B127" s="58"/>
       <c r="C127" s="58"/>
       <c r="D127" s="58"/>
@@ -8855,7 +8940,7 @@
         <v>122.56740557362289</v>
       </c>
     </row>
-    <row r="128" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B128" s="58"/>
       <c r="C128" s="58"/>
       <c r="D128" s="58"/>
@@ -8885,7 +8970,7 @@
         <v>127.40696510444312</v>
       </c>
     </row>
-    <row r="129" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B129" s="58"/>
       <c r="C129" s="58"/>
       <c r="D129" s="58"/>
@@ -8915,7 +9000,7 @@
         <v>132.6519938351399</v>
       </c>
     </row>
-    <row r="130" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B130" s="58"/>
       <c r="C130" s="58"/>
       <c r="D130" s="58"/>
@@ -8945,7 +9030,7 @@
         <v>138.3667737442475</v>
       </c>
     </row>
-    <row r="131" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B131" s="58"/>
       <c r="C131" s="58"/>
       <c r="D131" s="58"/>
@@ -8975,7 +9060,7 @@
         <v>144.63127594061237</v>
       </c>
     </row>
-    <row r="132" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B132" s="58"/>
       <c r="C132" s="58"/>
       <c r="D132" s="58"/>
@@ -9005,7 +9090,7 @@
         <v>151.54656182057519</v>
       </c>
     </row>
-    <row r="133" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B133" s="58"/>
       <c r="C133" s="58"/>
       <c r="D133" s="58"/>
@@ -9035,7 +9120,7 @@
         <v>159.24268114969374</v>
       </c>
     </row>
-    <row r="134" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B134" s="58"/>
       <c r="C134" s="58"/>
       <c r="D134" s="58"/>
@@ -9065,7 +9150,7 @@
         <v>167.89057371617793</v>
       </c>
     </row>
-    <row r="135" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B135" s="58"/>
       <c r="C135" s="58"/>
       <c r="D135" s="58"/>
@@ -9095,7 +9180,7 @@
         <v>177.72064885214024</v>
       </c>
     </row>
-    <row r="136" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B136" s="58"/>
       <c r="C136" s="58"/>
       <c r="D136" s="58"/>
@@ -9125,7 +9210,7 @@
         <v>189.05303858428945</v>
       </c>
     </row>
-    <row r="137" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B137" s="58"/>
       <c r="C137" s="58"/>
       <c r="D137" s="58"/>
@@ -9155,7 +9240,7 @@
         <v>202.34944935032485</v>
       </c>
     </row>
-    <row r="138" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B138" s="58"/>
       <c r="C138" s="58"/>
       <c r="D138" s="58"/>
@@ -9185,7 +9270,7 @@
         <v>218.30788190309138</v>
       </c>
     </row>
-    <row r="139" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B139" s="58"/>
       <c r="C139" s="58"/>
       <c r="D139" s="58"/>
@@ -9215,7 +9300,7 @@
         <v>238.05038961937979</v>
       </c>
     </row>
-    <row r="140" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B140" s="58"/>
       <c r="C140" s="58"/>
       <c r="D140" s="58"/>
@@ -9245,7 +9330,7 @@
         <v>263.5381222186993</v>
       </c>
     </row>
-    <row r="141" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B141" s="58"/>
       <c r="C141" s="58"/>
       <c r="D141" s="58"/>
@@ -9275,7 +9360,7 @@
         <v>298.6416948024189</v>
       </c>
     </row>
-    <row r="142" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B142" s="58"/>
       <c r="C142" s="58"/>
       <c r="D142" s="58"/>
@@ -9305,7 +9390,7 @@
         <v>352.64857159323731</v>
       </c>
     </row>
-    <row r="143" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B143" s="58"/>
       <c r="C143" s="58"/>
       <c r="D143" s="58"/>
@@ -9335,12 +9420,12 @@
         <v>458.27394232582373</v>
       </c>
     </row>
-    <row r="144" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:18" x14ac:dyDescent="0.4">
       <c r="O144" s="131"/>
       <c r="P144" s="199"/>
       <c r="Q144" s="198"/>
     </row>
-    <row r="145" spans="16:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="16:17" x14ac:dyDescent="0.4">
       <c r="P145" s="198"/>
       <c r="Q145" s="198"/>
     </row>
@@ -9374,35 +9459,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="0.44140625" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" customWidth="1"/>
+    <col min="1" max="1" width="0.41015625" customWidth="1"/>
+    <col min="2" max="2" width="3.64453125" customWidth="1"/>
+    <col min="3" max="3" width="22.64453125" customWidth="1"/>
+    <col min="4" max="4" width="9.3515625" customWidth="1"/>
+    <col min="5" max="5" width="8.52734375" customWidth="1"/>
+    <col min="6" max="6" width="8.3515625" customWidth="1"/>
+    <col min="7" max="7" width="8.1171875" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.1171875" customWidth="1"/>
+    <col min="10" max="10" width="8.64453125" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" customWidth="1"/>
-    <col min="14" max="14" width="0.5546875" customWidth="1"/>
-    <col min="15" max="15" width="1.88671875" customWidth="1"/>
+    <col min="13" max="13" width="10.1171875" customWidth="1"/>
+    <col min="14" max="14" width="0.52734375" customWidth="1"/>
+    <col min="15" max="15" width="1.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.35" x14ac:dyDescent="0.5">
       <c r="A1" s="17" t="s">
         <v>147</v>
       </c>
@@ -9419,7 +9504,7 @@
       <c r="L1" s="148"/>
       <c r="M1" s="148"/>
     </row>
-    <row r="2" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="149"/>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -9433,7 +9518,7 @@
       <c r="L2" s="148"/>
       <c r="M2" s="148"/>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="149"/>
       <c r="C3" s="150" t="s">
         <v>146</v>
@@ -9449,7 +9534,7 @@
       <c r="L3" s="148"/>
       <c r="M3" s="148"/>
     </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="4" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -9463,7 +9548,7 @@
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:14" s="4" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="4" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>100</v>
       </c>
@@ -9486,7 +9571,7 @@
       </c>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:14" s="4" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="4" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>103</v>
       </c>
@@ -9509,7 +9594,7 @@
       </c>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:14" s="4" customFormat="1" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="4" customFormat="1" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9"/>
       <c r="B7" s="128"/>
       <c r="C7" s="146"/>
@@ -9524,7 +9609,7 @@
       <c r="L7" s="196"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:14" s="4" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="4" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>101</v>
       </c>
@@ -9543,7 +9628,7 @@
       <c r="L8" s="258"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:14" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="4" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="146"/>
       <c r="C9" s="146"/>
       <c r="D9" s="9"/>
@@ -9557,7 +9642,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>128</v>
       </c>
@@ -9574,7 +9659,7 @@
       <c r="L10" s="61"/>
       <c r="M10" s="61"/>
     </row>
-    <row r="11" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="29"/>
       <c r="B11" s="2"/>
       <c r="C11" s="30"/>
@@ -9590,7 +9675,7 @@
       <c r="M11" s="16"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="31"/>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
@@ -9606,7 +9691,7 @@
       <c r="M12" s="22"/>
       <c r="N12" s="32"/>
     </row>
-    <row r="13" spans="1:14" s="23" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="23" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="31"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -9622,7 +9707,7 @@
       <c r="M13" s="22"/>
       <c r="N13" s="32"/>
     </row>
-    <row r="14" spans="1:14" s="23" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="23" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="31"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -9638,7 +9723,7 @@
       <c r="M14" s="22"/>
       <c r="N14" s="32"/>
     </row>
-    <row r="15" spans="1:14" s="23" customFormat="1" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="23" customFormat="1" ht="7.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="31"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
@@ -9654,7 +9739,7 @@
       <c r="M15" s="22"/>
       <c r="N15" s="32"/>
     </row>
-    <row r="16" spans="1:14" s="23" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="23" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="35"/>
@@ -9670,7 +9755,7 @@
       <c r="M16" s="35"/>
       <c r="N16" s="36"/>
     </row>
-    <row r="17" spans="1:14" s="23" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="23" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="60"/>
       <c r="C17" s="61"/>
       <c r="D17" s="61"/>
@@ -9684,7 +9769,7 @@
       <c r="L17" s="61"/>
       <c r="M17" s="22"/>
     </row>
-    <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="47" t="s">
         <v>144</v>
       </c>
@@ -9701,7 +9786,7 @@
       <c r="L18" s="61"/>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="51"/>
       <c r="B19" s="55"/>
       <c r="C19" s="55"/>
@@ -9717,7 +9802,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="41"/>
       <c r="B20" s="144" t="s">
         <v>112</v>
@@ -9748,7 +9833,7 @@
       </c>
       <c r="N20" s="6"/>
     </row>
-    <row r="21" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="31"/>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
@@ -9764,7 +9849,7 @@
       <c r="M21" s="22"/>
       <c r="N21" s="32"/>
     </row>
-    <row r="22" spans="1:14" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="31"/>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
@@ -9780,7 +9865,7 @@
       <c r="M22" s="22"/>
       <c r="N22" s="32"/>
     </row>
-    <row r="23" spans="1:14" s="23" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="23" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="31"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
@@ -9796,7 +9881,7 @@
       <c r="M23" s="22"/>
       <c r="N23" s="32"/>
     </row>
-    <row r="24" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="31"/>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
@@ -9812,7 +9897,7 @@
       <c r="M24" s="22"/>
       <c r="N24" s="32"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="41"/>
       <c r="B25" s="60"/>
       <c r="C25" s="143" t="s">
@@ -9830,7 +9915,7 @@
       <c r="M25" s="14"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="26" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="41"/>
       <c r="B26" s="70" t="s">
         <v>136</v>
@@ -9865,7 +9950,7 @@
       </c>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="31"/>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
@@ -9881,7 +9966,7 @@
       <c r="M27" s="22"/>
       <c r="N27" s="32"/>
     </row>
-    <row r="28" spans="1:14" s="23" customFormat="1" ht="83.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="23" customFormat="1" ht="83.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="31"/>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
@@ -9897,7 +9982,7 @@
       <c r="M28" s="22"/>
       <c r="N28" s="32"/>
     </row>
-    <row r="29" spans="1:14" s="23" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="23" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="31"/>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
@@ -9913,7 +9998,7 @@
       <c r="M29" s="22"/>
       <c r="N29" s="32"/>
     </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="41"/>
       <c r="B30" s="60"/>
       <c r="C30" s="140" t="s">
@@ -9931,7 +10016,7 @@
       <c r="M30" s="61"/>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="41"/>
       <c r="B31" s="70" t="s">
         <v>137</v>
@@ -9964,7 +10049,7 @@
       </c>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="31"/>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
@@ -9980,7 +10065,7 @@
       <c r="M32" s="22"/>
       <c r="N32" s="32"/>
     </row>
-    <row r="33" spans="1:14" s="23" customFormat="1" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="23" customFormat="1" ht="31.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="31"/>
       <c r="B33" s="21"/>
       <c r="C33" s="22"/>
@@ -9996,7 +10081,7 @@
       <c r="M33" s="22"/>
       <c r="N33" s="32"/>
     </row>
-    <row r="34" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="31"/>
       <c r="B34" s="21"/>
       <c r="C34" s="22"/>
@@ -10012,7 +10097,7 @@
       <c r="M34" s="22"/>
       <c r="N34" s="32"/>
     </row>
-    <row r="35" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="41"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14"/>
@@ -10028,7 +10113,7 @@
       <c r="M35" s="14"/>
       <c r="N35" s="6"/>
     </row>
-    <row r="36" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="41"/>
       <c r="B36" s="70" t="s">
         <v>138</v>
@@ -10059,7 +10144,7 @@
       </c>
       <c r="N36" s="6"/>
     </row>
-    <row r="37" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="31"/>
       <c r="B37" s="21"/>
       <c r="C37" s="22"/>
@@ -10077,7 +10162,7 @@
       </c>
       <c r="N37" s="32"/>
     </row>
-    <row r="38" spans="1:14" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="31"/>
       <c r="B38" s="21"/>
       <c r="C38" s="22"/>
@@ -10093,7 +10178,7 @@
       <c r="M38" s="22"/>
       <c r="N38" s="32"/>
     </row>
-    <row r="39" spans="1:14" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="31"/>
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
@@ -10109,7 +10194,7 @@
       <c r="M39" s="22"/>
       <c r="N39" s="32"/>
     </row>
-    <row r="40" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="41"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
@@ -10125,7 +10210,7 @@
       <c r="M40" s="14"/>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="41"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
@@ -10141,7 +10226,7 @@
       <c r="M41" s="14"/>
       <c r="N41" s="6"/>
     </row>
-    <row r="42" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="41"/>
       <c r="B42" s="70" t="s">
         <v>134</v>
@@ -10172,7 +10257,7 @@
       </c>
       <c r="N42" s="6"/>
     </row>
-    <row r="43" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="31"/>
       <c r="B43" s="21"/>
       <c r="C43" s="22"/>
@@ -10188,7 +10273,7 @@
       <c r="M43" s="22"/>
       <c r="N43" s="32"/>
     </row>
-    <row r="44" spans="1:14" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="31"/>
       <c r="B44" s="21"/>
       <c r="C44" s="22"/>
@@ -10204,7 +10289,7 @@
       <c r="M44" s="22"/>
       <c r="N44" s="32"/>
     </row>
-    <row r="45" spans="1:14" s="23" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="23" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="31"/>
       <c r="B45" s="21"/>
       <c r="C45" s="22"/>
@@ -10220,7 +10305,7 @@
       <c r="M45" s="22"/>
       <c r="N45" s="32"/>
     </row>
-    <row r="46" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="42"/>
       <c r="B46" s="10"/>
       <c r="C46" s="15"/>
@@ -10236,7 +10321,7 @@
       <c r="M46" s="15"/>
       <c r="N46" s="24"/>
     </row>
-    <row r="47" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
@@ -10250,7 +10335,7 @@
       <c r="L47" s="14"/>
       <c r="M47" s="14"/>
     </row>
-    <row r="48" spans="1:14" s="49" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="49" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="48" t="s">
         <v>149</v>
       </c>
@@ -10267,7 +10352,7 @@
       <c r="L48" s="152"/>
       <c r="M48" s="152"/>
     </row>
-    <row r="49" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="40"/>
       <c r="B49" s="46"/>
       <c r="C49" s="16"/>
@@ -10283,7 +10368,7 @@
       <c r="M49" s="16"/>
       <c r="N49" s="5"/>
     </row>
-    <row r="50" spans="1:14" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="41"/>
       <c r="B50" s="61"/>
       <c r="C50" s="153"/>
@@ -10308,7 +10393,7 @@
       <c r="M50" s="153"/>
       <c r="N50" s="6"/>
     </row>
-    <row r="51" spans="1:14" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="41"/>
       <c r="B51" s="156" t="s">
         <v>145</v>
@@ -10333,7 +10418,7 @@
       <c r="M51" s="153"/>
       <c r="N51" s="6"/>
     </row>
-    <row r="52" spans="1:14" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A52" s="41"/>
       <c r="B52" s="159"/>
       <c r="C52" s="160" t="s">
@@ -10358,7 +10443,7 @@
       <c r="M52" s="153"/>
       <c r="N52" s="6"/>
     </row>
-    <row r="53" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" s="41"/>
       <c r="B53" s="163"/>
       <c r="C53" s="164" t="s">
@@ -10386,7 +10471,7 @@
       <c r="M53" s="155"/>
       <c r="N53" s="6"/>
     </row>
-    <row r="54" spans="1:14" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A54" s="41"/>
       <c r="B54" s="163"/>
       <c r="C54" s="167" t="s">
@@ -10416,7 +10501,7 @@
       <c r="M54" s="155"/>
       <c r="N54" s="6"/>
     </row>
-    <row r="55" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="41"/>
       <c r="B55" s="163"/>
       <c r="C55" s="167" t="s">
@@ -10441,7 +10526,7 @@
       <c r="M55" s="155"/>
       <c r="N55" s="6"/>
     </row>
-    <row r="56" spans="1:14" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A56" s="41"/>
       <c r="B56" s="163"/>
       <c r="C56" s="171"/>
@@ -10466,7 +10551,7 @@
       </c>
       <c r="N56" s="6"/>
     </row>
-    <row r="57" spans="1:14" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A57" s="41"/>
       <c r="B57" s="163"/>
       <c r="C57" s="173" t="s">
@@ -10498,7 +10583,7 @@
       </c>
       <c r="N57" s="6"/>
     </row>
-    <row r="58" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="41"/>
       <c r="B58" s="163"/>
       <c r="C58" s="175" t="s">
@@ -10523,7 +10608,7 @@
       </c>
       <c r="N58" s="6"/>
     </row>
-    <row r="59" spans="1:14" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A59" s="41"/>
       <c r="B59" s="178"/>
       <c r="C59" s="179" t="s">
@@ -10544,7 +10629,7 @@
       <c r="M59" s="155"/>
       <c r="N59" s="6"/>
     </row>
-    <row r="60" spans="1:14" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="41"/>
       <c r="B60" s="153"/>
       <c r="C60" s="153"/>
@@ -10574,7 +10659,7 @@
       </c>
       <c r="N60" s="6"/>
     </row>
-    <row r="61" spans="1:14" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A61" s="41"/>
       <c r="B61" s="153"/>
       <c r="C61" s="153"/>
@@ -10594,7 +10679,7 @@
       </c>
       <c r="N61" s="6"/>
     </row>
-    <row r="62" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="41"/>
       <c r="B62" s="153"/>
       <c r="C62" s="153"/>
@@ -10614,7 +10699,7 @@
       </c>
       <c r="N62" s="6"/>
     </row>
-    <row r="63" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="41"/>
       <c r="B63" s="153"/>
       <c r="C63" s="153"/>
@@ -10630,7 +10715,7 @@
       <c r="M63" s="155"/>
       <c r="N63" s="6"/>
     </row>
-    <row r="64" spans="1:14" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A64" s="41"/>
       <c r="B64" s="153"/>
       <c r="C64" s="153"/>
@@ -10656,7 +10741,7 @@
       </c>
       <c r="N64" s="6"/>
     </row>
-    <row r="65" spans="1:20" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A65" s="41"/>
       <c r="B65" s="153"/>
       <c r="C65" s="153"/>
@@ -10676,7 +10761,7 @@
       </c>
       <c r="N65" s="6"/>
     </row>
-    <row r="66" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="41"/>
       <c r="B66" s="182" t="s">
         <v>84</v>
@@ -10698,7 +10783,7 @@
       </c>
       <c r="N66" s="6"/>
     </row>
-    <row r="67" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="42"/>
       <c r="B67" s="12"/>
       <c r="C67" s="43"/>
@@ -10714,7 +10799,7 @@
       <c r="M67" s="43"/>
       <c r="N67" s="24"/>
     </row>
-    <row r="68" spans="1:20" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B68" s="13"/>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
@@ -10728,7 +10813,7 @@
       <c r="L68" s="14"/>
       <c r="M68" s="14"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.4">
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
@@ -10764,1392 +10849,1392 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="93.109375" customWidth="1"/>
+    <col min="1" max="1" width="93.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="207" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="231" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="207" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="208" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="209"/>
     </row>
-    <row r="6" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="210" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="210" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="210" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="210" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="211" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="212" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="213" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="211" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="6.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="214"/>
     </row>
-    <row r="15" spans="1:1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="215"/>
     </row>
-    <row r="16" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="216" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="215"/>
     </row>
-    <row r="18" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="217" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="217" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="217" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="217" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="66" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="224" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="318" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="318" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="224"/>
     </row>
-    <row r="24" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="218" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="219" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="39.299999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="39.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="228" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="36.299999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="36.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="219" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="228" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="229" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="46.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="229" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="47.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="229" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="7.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="229"/>
     </row>
-    <row r="33" spans="1:1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="220"/>
     </row>
-    <row r="34" spans="1:1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="215"/>
     </row>
-    <row r="35" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="216" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="217" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="217" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="224" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="216" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="216" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="217" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="217" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="217" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="217" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" ht="45.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="217" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="221" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="216" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="217" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="217" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="217" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="47.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="222" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="217"/>
     </row>
-    <row r="53" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="216" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="218" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="217" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="224" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="224" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="224" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="224" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="224" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="224" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" ht="37.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="224" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" ht="46.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="224" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="224" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="31.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="224" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="224" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="46.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="224" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="224" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="224" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="217" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="227" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="224" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="30.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="224" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" ht="19.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="224" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" ht="31.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="224" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" ht="19.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="224" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="227" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="19.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="224" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A79" s="224" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" ht="31.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" s="224" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A81" s="224" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A82" s="224" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A83" s="227" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A84" s="217" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A85" s="217" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A86" s="217" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="31.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A87" s="217" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="42.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A88" s="217" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A89" s="217" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A90" s="217" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="217" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A92" s="222" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A93" s="222" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A94" s="216" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A95" s="221" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A96" s="221" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="221" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" s="221" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A99" s="221" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="221" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A101" s="221" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A102" s="221" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A103" s="221" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A104" s="221" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A105" s="221" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A106" s="216" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="221" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="221" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="221" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A110" s="216" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A111" s="221" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="221" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A113" s="221" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A114" s="221" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A115" s="221" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A116" s="221" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A117" s="222" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A118" s="222" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A119" s="216" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A120" s="221" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A121" s="221" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A122" s="221" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A123" s="221" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A124" s="221" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A125" s="221" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A126" s="221" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A127" s="221" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A128" s="221" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A129" s="221" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="130" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A130" s="216" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A131" s="217" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A132" s="217" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A133" s="217" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A134" s="217" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A135" s="222" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A136" s="217" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A137" s="216" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A138" s="217" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A139" s="217" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A140" s="217" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A141" s="217" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A142" s="217" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A143" s="217" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A144" s="217" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A145" s="217" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A146" s="217" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A147" s="222" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" ht="31.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A148" s="216" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="149" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A149" s="217" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A150" s="224" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A151" s="217" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A152" s="217" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A153" s="222" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A154" s="223" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A155" s="216" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" ht="48" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="217" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A157" s="217" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A158" s="217" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A159" s="217" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" ht="51.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A160" s="217" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A161" s="217" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A162" s="217" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" ht="48" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A163" s="217" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A164" s="224" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="165" spans="1:1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A165" s="217" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A166" s="217" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A167" s="222"/>
     </row>
-    <row r="168" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A168" s="216" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A169" s="221" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="170" spans="1:1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A170" s="221" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A171" s="221" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A172" s="217" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="173" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A173" s="217" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A174" s="216" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" ht="46.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A175" s="224" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A176" s="224" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A177" s="217" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" ht="36.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A178" s="217" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A179" s="217" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="180" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A180" s="224" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A181" s="217" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A182" s="217" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A183" s="217" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" ht="46.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A184" s="217" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" ht="8.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A185" s="219"/>
     </row>
-    <row r="186" spans="1:1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A186" s="225"/>
     </row>
-    <row r="187" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A187" s="216" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A188" s="226" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A189" s="217" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A190" s="224" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A191" s="224" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A192" s="217" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" ht="33.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A193" s="217" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A194" s="221" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="195" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A195" s="221" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A196" s="221" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A197" s="221" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A198" s="217" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A199" s="217" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="200" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A200" s="217" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="201" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A201" s="217" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A202" s="217"/>
     </row>
-    <row r="203" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A203" s="216" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="204" spans="1:1" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" ht="43.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A204" s="224" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="205" spans="1:1" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A205" s="224" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="206" spans="1:1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" ht="45.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A206" s="224" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="207" spans="1:1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" ht="45.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A207" s="224" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="208" spans="1:1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" ht="45.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A208" s="230" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="209" spans="1:1" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" ht="43.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A209" s="224" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="210" spans="1:1" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" ht="44.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A210" s="228" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="211" spans="1:1" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" ht="31.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A211" s="224" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="212" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A212" s="229" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="213" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A213" s="229" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="214" spans="1:1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A214" s="229" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="215" spans="1:1" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" ht="57.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A215" s="224" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="216" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A216" s="216" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="217" spans="1:1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A217" s="207"/>
     </row>
-    <row r="218" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A218" s="216" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="219" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A219" s="217" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="220" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A220" s="217" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="221" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A221" s="217" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="222" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A222" s="217" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="223" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A223" s="217" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="224" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A224" s="216" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="225" spans="1:1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A225" s="217" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A226" s="217" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="227" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A227" s="217" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="228" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A228" s="217" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="229" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A229" s="217" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="230" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A230" s="217" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="231" spans="1:1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" ht="9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A231" s="217"/>
     </row>
-    <row r="232" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A232" s="216" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="233" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A233" s="217" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="234" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A234" s="217" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="235" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A235" s="221" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="236" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A236" s="221" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="237" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A237" s="221" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="238" spans="1:1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A238" s="221" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="239" spans="1:1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A239" s="221" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="240" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A240" s="221" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="241" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A241" s="221" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="242" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A242" s="221" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="243" spans="1:1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" ht="48.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A243" s="221" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="244" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A244" s="221" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="245" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A245" s="221" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A246" s="217"/>
     </row>
-    <row r="247" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A247" s="216" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="248" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A248" s="221" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="249" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A249" s="221" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="250" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A250" s="221" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="251" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A251" s="221" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="252" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A252" s="221" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A253" s="217" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="254" spans="1:1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A254" s="217"/>
     </row>
-    <row r="255" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A255" s="227" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="256" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A256" s="217" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="257" spans="1:1" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" ht="44.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A257" s="224" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="258" spans="1:1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A258" s="221" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="259" spans="1:1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A259" s="217" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="260" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A260" s="217" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="261" spans="1:1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A261" s="217" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A262" s="217" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="263" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A263" s="217" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" ht="9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A264" s="217"/>
     </row>
-    <row r="265" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A265" s="227" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="266" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A266" s="217" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="267" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A267" s="224" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="268" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A268" s="217" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="269" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A269" s="224" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="270" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A270" s="224" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="271" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" ht="49.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A271" s="224" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A272" s="133"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A273" s="133"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A274" s="133"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A275" s="133"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A276" s="133"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A277" s="133"/>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A278" s="133"/>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A279" s="133"/>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A280" s="133"/>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A281" s="133"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A282" s="133"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A283" s="133"/>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A284" s="133"/>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A285" s="133"/>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A286" s="133"/>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A287" s="133"/>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A288" s="133"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A289" s="133"/>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A290" s="133"/>
     </row>
   </sheetData>

</xml_diff>